<commit_message>
SMART_RADAR_WEBAPP.V1.1.2-ALPHA - add is_show_corporate
</commit_message>
<xml_diff>
--- a/see-kpi-portlet/docroot/file/import_employee_template.xlsx
+++ b/see-kpi-portlet/docroot/file/import_employee_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOTO\git\see-kpi-portlet\docroot\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toto\git\see-kpi-portlet-ghb\see-kpi-portlet\docroot\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{79F6C009-D9A7-410A-9ECB-B7A7919FE4F4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595" tabRatio="798"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8595" tabRatio="798" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Employee Code</t>
   </si>
@@ -63,12 +64,15 @@
   </si>
   <si>
     <t>Has Second Line</t>
+  </si>
+  <si>
+    <t>Is Show Corporate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -429,11 +433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -451,11 +455,12 @@
     <col min="11" max="11" width="14" style="2"/>
     <col min="12" max="12" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="1000" width="11.28515625" style="2"/>
+    <col min="14" max="14" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="1000" width="11.28515625" style="2"/>
     <col min="1001" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,6 +499,9 @@
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>